<commit_message>
update: py code and pdfs
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/econ/week1/week1-win.xlsx
+++ b/PM2/econ/week1/week1-win.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\econ\week1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5264D2EE-8E7A-4E9F-8E4E-461A9ACE03E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A1597A-4B7E-4C2C-B031-6ABAB7C4E35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valor Futuro" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>tasa/costo de oportunidad</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ej </t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>hoy</t>
+  </si>
+  <si>
+    <t>1 año</t>
   </si>
 </sst>
 </file>
@@ -1494,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2424,10 +2433,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEDD708-FB60-4AFC-B160-D336DC608D69}">
-  <dimension ref="A3:F20"/>
+  <dimension ref="A3:F27"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2570,6 +2579,57 @@
         <v>15709.376534118803</v>
       </c>
     </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f>1*(1+16.8%)</f>
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="D24">
+        <f>16.8/12</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f>B25*(1+1.4%)^(360)</f>
+        <v>149.16392378391404</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="4">
+        <v>4.32275595605619E-4</v>
+      </c>
+      <c r="D27">
+        <f>B24*(1+C27)^(360)</f>
+        <v>1.1683419289046044</v>
+      </c>
+      <c r="E27">
+        <f>16.8/12</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>